<commit_message>
feat: implement preinscritos export/report system with modal chooser
- Add ExportController with report generation, Excel export and file download
- Create Exportacion model for tracking exports in database
- Implement ReportePresritoService for filter processing
- Add PresritosExport class for Excel format generation
- Create reportes view with filters, statistics, modal chooser and File System API
- Implement dual-option workflow: DB-only vs DB + Excel generation
- Add SweetAlert2 integration for user feedback
- Fix JSON escaping in Blade templates using @json() helper
- Add sidebar menu entries for preinscritos reports
- Clear compiled views cache
</commit_message>
<xml_diff>
--- a/pre incripciones.xlsx
+++ b/pre incripciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AdminSena\Documents\SoeSoftware2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1829B70A-6E8F-445D-B63A-A954EB5B0D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189D3728-24E9-47F9-9FA1-45F0FB35E0B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2067,7 +2067,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>